<commit_message>
Compare doubles 255.0 against 255
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -274,19 +274,19 @@
                   <c:v>Dart VM (checked mode) on Dartium</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>dart2js on Chrome</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>TypeScript to Javascript on Explorer</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>C# to javascript on Explorer</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>dart2js on Chrome</c:v>
-                </c:pt>
                 <c:pt idx="10">
+                  <c:v>dart2js on Explorer</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>dart2js on Firefox</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>dart2js on Explorer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -301,7 +301,7 @@
                   <c:v>8.3179999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.872</c:v>
+                  <c:v>10.111000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16.145</c:v>
@@ -316,22 +316,22 @@
                   <c:v>26.873999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.09</c:v>
+                  <c:v>27.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>35.323</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>57.438000000000002</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>60.642000000000003</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>122.13800000000001</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>496.00900000000001</c:v>
+                  <c:v>212.096</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>533.577</c:v>
+                  <c:v>218.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,11 +346,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="179651440"/>
-        <c:axId val="179652000"/>
+        <c:axId val="132295552"/>
+        <c:axId val="132296112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="179651440"/>
+        <c:axId val="132295552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +393,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179652000"/>
+        <c:crossAx val="132296112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -401,7 +401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179652000"/>
+        <c:axId val="132296112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +452,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179651440"/>
+        <c:crossAx val="132295552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="10"/>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,11 +1385,11 @@
         <v>6</v>
       </c>
       <c r="C2" t="str">
-        <f>A2&amp; " on "&amp;B2</f>
+        <f t="shared" ref="C2:C13" si="0">A2&amp; " on "&amp;B2</f>
         <v>TypeScript to Javascript on Chrome</v>
       </c>
       <c r="D2" s="3">
-        <f>E2/1000</f>
+        <f t="shared" ref="D2:D13" si="1">E2/1000</f>
         <v>8.3179999999999996</v>
       </c>
       <c r="E2">
@@ -1404,15 +1404,15 @@
         <v>0</v>
       </c>
       <c r="C3" t="str">
-        <f>A3&amp; " on "&amp;B3</f>
+        <f t="shared" si="0"/>
         <v>Dart VM (unchecked mode) on Dartium</v>
       </c>
       <c r="D3" s="3">
-        <f>E3/1000</f>
-        <v>12.872</v>
+        <f t="shared" si="1"/>
+        <v>10.111000000000001</v>
       </c>
       <c r="E3">
-        <v>12872</v>
+        <v>10111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,11 +1423,11 @@
         <v>6</v>
       </c>
       <c r="C4" t="str">
-        <f>A4&amp; " on "&amp;B4</f>
+        <f t="shared" si="0"/>
         <v>C# to javascript on Chrome</v>
       </c>
       <c r="D4" s="3">
-        <f>E4/1000</f>
+        <f t="shared" si="1"/>
         <v>16.145</v>
       </c>
       <c r="E4">
@@ -1442,11 +1442,11 @@
         <v>12</v>
       </c>
       <c r="C5" t="str">
-        <f>A5&amp; " on "&amp;B5</f>
+        <f t="shared" si="0"/>
         <v>MSIL (C# native) on Windows</v>
       </c>
       <c r="D5" s="3">
-        <f>E5/1000</f>
+        <f t="shared" si="1"/>
         <v>17.524999999999999</v>
       </c>
       <c r="E5">
@@ -1461,11 +1461,11 @@
         <v>5</v>
       </c>
       <c r="C6" t="str">
-        <f>A6&amp; " on "&amp;B6</f>
+        <f t="shared" si="0"/>
         <v>TypeScript to Javascript on Firefox</v>
       </c>
       <c r="D6" s="3">
-        <f>E6/1000</f>
+        <f t="shared" si="1"/>
         <v>24.289000000000001</v>
       </c>
       <c r="E6">
@@ -1480,11 +1480,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="str">
-        <f>A7&amp; " on "&amp;B7</f>
+        <f t="shared" si="0"/>
         <v>C# to javascript on Firefox</v>
       </c>
       <c r="D7" s="3">
-        <f>E7/1000</f>
+        <f t="shared" si="1"/>
         <v>26.873999999999999</v>
       </c>
       <c r="E7">
@@ -1499,72 +1499,72 @@
         <v>0</v>
       </c>
       <c r="C8" t="str">
-        <f>A8&amp; " on "&amp;B8</f>
+        <f t="shared" si="0"/>
         <v>Dart VM (checked mode) on Dartium</v>
       </c>
       <c r="D8" s="3">
-        <f>E8/1000</f>
-        <v>30.09</v>
+        <f t="shared" si="1"/>
+        <v>27.3</v>
       </c>
       <c r="E8">
-        <v>30090</v>
+        <v>27300</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9" t="str">
-        <f>A9&amp; " on "&amp;B9</f>
-        <v>TypeScript to Javascript on Explorer</v>
+        <f t="shared" si="0"/>
+        <v>dart2js on Chrome</v>
       </c>
       <c r="D9" s="3">
-        <f>E9/1000</f>
-        <v>57.438000000000002</v>
+        <f t="shared" si="1"/>
+        <v>35.323</v>
       </c>
       <c r="E9">
-        <v>57438</v>
+        <v>35323</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="str">
-        <f>A10&amp; " on "&amp;B10</f>
-        <v>C# to javascript on Explorer</v>
+        <f t="shared" si="0"/>
+        <v>TypeScript to Javascript on Explorer</v>
       </c>
       <c r="D10" s="3">
-        <f>E10/1000</f>
-        <v>60.642000000000003</v>
+        <f t="shared" si="1"/>
+        <v>57.438000000000002</v>
       </c>
       <c r="E10">
-        <v>60642</v>
+        <v>57438</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="str">
-        <f>A11&amp; " on "&amp;B11</f>
-        <v>dart2js on Chrome</v>
+        <f t="shared" si="0"/>
+        <v>C# to javascript on Explorer</v>
       </c>
       <c r="D11" s="3">
-        <f>E11/1000</f>
-        <v>122.13800000000001</v>
+        <f t="shared" si="1"/>
+        <v>60.642000000000003</v>
       </c>
       <c r="E11">
-        <v>122138</v>
+        <v>60642</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,18 +1572,18 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" t="str">
-        <f>A12&amp; " on "&amp;B12</f>
-        <v>dart2js on Firefox</v>
+        <f t="shared" si="0"/>
+        <v>dart2js on Explorer</v>
       </c>
       <c r="D12" s="3">
-        <f>E12/1000</f>
-        <v>496.00900000000001</v>
+        <f t="shared" si="1"/>
+        <v>212.096</v>
       </c>
       <c r="E12">
-        <v>496009</v>
+        <v>212096</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,18 +1591,18 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" t="str">
-        <f>A13&amp; " on "&amp;B13</f>
-        <v>dart2js on Explorer</v>
+        <f t="shared" si="0"/>
+        <v>dart2js on Firefox</v>
       </c>
       <c r="D13" s="3">
-        <f>E13/1000</f>
-        <v>533.577</v>
+        <f t="shared" si="1"/>
+        <v>218.93</v>
       </c>
       <c r="E13">
-        <v>533577</v>
+        <v>218930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>